<commit_message>
SE and Part of NE added to grundy urls
</commit_message>
<xml_diff>
--- a/complete links/Grundy_url_files/se Grundy urls.xlsx
+++ b/complete links/Grundy_url_files/se Grundy urls.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d7eead86a347b36d/Desktop/Summer DPSG/DSPG2023/Housing/HousingDatabase/complete links/Grundy_url_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="8_{484D0590-74B7-4629-B04E-7A178DD1EF4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{994A74B2-2736-4FC8-9B8F-229BCDF61D74}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="8_{484D0590-74B7-4629-B04E-7A178DD1EF4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{85CC1B85-C668-4A65-B5AE-6E70C39FE981}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{27D08D04-FB51-4D03-BB32-EF6749594A24}"/>
   </bookViews>
@@ -1104,18 +1104,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1138,16 +1130,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1161,6 +1151,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1462,8 +1456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADAAC839-5404-4046-A337-88C21327567B}">
   <dimension ref="A1:G351"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A332" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G351"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -8139,11 +8133,7 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1" xr:uid="{48A9A0BE-2BE9-4E72-B220-C7217003CBFF}"/>
-    <hyperlink ref="F2" r:id="rId2" xr:uid="{D66C3806-AAA4-4F55-992F-072CCF14D2D4}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>